<commit_message>
Absolute magnitudes for each luminosity class
TODO: import data
</commit_message>
<xml_diff>
--- a/Authorative Table.xlsx
+++ b/Authorative Table.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNITY\Orbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BEE047-1FA9-455F-8FA6-5AC64A95FBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD17515-CE7A-48DA-8230-F333D041509A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F9C6455-CBDE-45B2-AE91-212659DAF4F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F9C6455-CBDE-45B2-AE91-212659DAF4F4}"/>
   </bookViews>
   <sheets>
-    <sheet name="table" sheetId="1" r:id="rId1"/>
+    <sheet name="bolometric correction" sheetId="1" r:id="rId1"/>
+    <sheet name="absolute magnitudes" sheetId="2" r:id="rId2"/>
+    <sheet name="main-sequence stars" sheetId="5" r:id="rId3"/>
+    <sheet name="giants" sheetId="3" r:id="rId4"/>
+    <sheet name="supergiants" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
   <si>
     <t>Spectral Type</t>
   </si>
@@ -243,13 +247,304 @@
   </si>
   <si>
     <t xml:space="preserve">M9V   </t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>O4</t>
+  </si>
+  <si>
+    <t>O5</t>
+  </si>
+  <si>
+    <t>O6</t>
+  </si>
+  <si>
+    <t>O7</t>
+  </si>
+  <si>
+    <t>O8</t>
+  </si>
+  <si>
+    <t>Spectral Class</t>
+  </si>
+  <si>
+    <t>VBc1</t>
+  </si>
+  <si>
+    <t>VBc2</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>VBc range of classes</t>
+  </si>
+  <si>
+    <t>VBc of spectral types</t>
+  </si>
+  <si>
+    <t>totalbc</t>
+  </si>
+  <si>
+    <t>typebc</t>
+  </si>
+  <si>
+    <t>Luminosity (in solar luminosities)</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>M8</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spectral Type </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature (K) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute Magnitude </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">O9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">G8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">K7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* </t>
+  </si>
+  <si>
+    <t>Mv1</t>
+  </si>
+  <si>
+    <t>Mv2</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Main-sequence stars</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>M9</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Supergiants</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>ű</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,16 +553,38 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -275,12 +592,557 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -354,7 +1216,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>table!$C$1</c:f>
+              <c:f>'bolometric correction'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -375,7 +1237,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>table!$A$2:$A$67</c:f>
+              <c:f>'bolometric correction'!$A$10:$A$75</c:f>
               <c:strCache>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
@@ -581,7 +1443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>table!$C$2:$C$67</c:f>
+              <c:f>'bolometric correction'!$C$10:$C$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -1566,16 +2428,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1900,10 +2762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB801A8-3ECF-4FE2-92E5-82FBD989E008}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1911,749 +2773,3072 @@
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="F1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="F2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17">
+        <v>-4.7474999999999996</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-4.8</v>
+      </c>
+      <c r="H3" s="5">
+        <v>-3.06</v>
+      </c>
+      <c r="I3">
+        <f>H3-G3</f>
+        <v>1.7399999999999998</v>
+      </c>
+      <c r="J3">
+        <f>I3/8</f>
+        <v>0.21749999999999997</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20">
+        <v>-4.5459523809523796</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-3.03</v>
+      </c>
+      <c r="H4" s="5">
+        <v>-0.38</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I9" si="0">H4-G4</f>
+        <v>2.65</v>
+      </c>
+      <c r="J4">
+        <f>I4/10</f>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L9" si="1">G4+K4*J4</f>
+        <v>-2.7649999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20">
+        <v>-4.3444047619047703</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-0.24</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J9" si="2">I5/10</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>-0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20">
+        <v>-4.1428571428571397</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="H6" s="5">
+        <v>-0.08</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>-7.000000000000001E-3</v>
+      </c>
+      <c r="K6">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>-3.1000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20">
+        <v>-3.9413095238095202</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-0.09</v>
+      </c>
+      <c r="H7" s="5">
+        <v>-0.21</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>-0.12</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>-1.2E-2</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>-0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20">
+        <v>-3.7397619047619002</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-0.22</v>
+      </c>
+      <c r="H8" s="5">
+        <v>-1.25</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>-1.03</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>-0.10300000000000001</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20">
+        <v>-3.53821428571429</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="7">
+        <v>-1.3</v>
+      </c>
+      <c r="H9" s="8">
+        <v>-5.73</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>-4.4300000000000006</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>-0.44300000000000006</v>
+      </c>
+      <c r="K9">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>-5.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="19">
         <v>34000</v>
       </c>
-      <c r="C2">
+      <c r="C10" s="20">
         <v>-3.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B11" s="19">
         <v>32000</v>
       </c>
-      <c r="C3">
+      <c r="C11" s="20">
         <v>-3.06</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B12" s="19">
         <v>31500</v>
       </c>
-      <c r="C4">
+      <c r="C12" s="20">
         <v>-3.03</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B13" s="19">
         <v>29000</v>
       </c>
-      <c r="C5">
+      <c r="C13" s="20">
         <v>-2.87</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B14" s="19">
         <v>26000</v>
       </c>
-      <c r="C6">
+      <c r="C14" s="20">
         <v>-2.61</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B15" s="19">
         <v>24800</v>
       </c>
-      <c r="C7">
+      <c r="C15" s="20">
         <v>-2.4300000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B16" s="19">
         <v>20600</v>
       </c>
-      <c r="C8">
+      <c r="C16" s="20">
         <v>-2.06</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B17" s="19">
         <v>18500</v>
       </c>
-      <c r="C9">
+      <c r="C17" s="20">
         <v>-1.79</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B18" s="19">
         <v>17000</v>
       </c>
-      <c r="C10">
+      <c r="C18" s="20">
         <v>-1.58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B19" s="19">
         <v>16700</v>
       </c>
-      <c r="C11">
+      <c r="C19" s="20">
         <v>-1.53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B20" s="19">
         <v>15700</v>
       </c>
-      <c r="C12">
+      <c r="C20" s="20">
         <v>-1.37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
+      <c r="B21" s="19">
         <v>14500</v>
       </c>
-      <c r="C13">
+      <c r="C21" s="20">
         <v>-1.1599999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
+      <c r="B22" s="19">
         <v>14000</v>
       </c>
-      <c r="C14">
+      <c r="C22" s="20">
         <v>-1.07</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B15">
+      <c r="B23" s="19">
         <v>12500</v>
       </c>
-      <c r="C15">
+      <c r="C23" s="20">
         <v>-0.79</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B16">
+      <c r="B24" s="19">
         <v>10700</v>
       </c>
-      <c r="C16">
+      <c r="C24" s="20">
         <v>-0.44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B17">
+      <c r="B25" s="19">
         <v>10400</v>
       </c>
-      <c r="C17">
+      <c r="C25" s="20">
         <v>-0.38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
+      <c r="B26" s="19">
         <v>9700</v>
       </c>
-      <c r="C18">
+      <c r="C26" s="20">
         <v>-0.24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B19">
+      <c r="B27" s="19">
         <v>9200</v>
       </c>
-      <c r="C19">
+      <c r="C27" s="20">
         <v>-0.15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B20">
+      <c r="B28" s="19">
         <v>8840</v>
       </c>
-      <c r="C20">
+      <c r="C28" s="20">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B21">
+      <c r="B29" s="19">
         <v>8550</v>
       </c>
-      <c r="C21">
+      <c r="C29" s="20">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B22">
+      <c r="B30" s="19">
         <v>8270</v>
       </c>
-      <c r="C22">
+      <c r="C30" s="20">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B23">
+      <c r="B31" s="19">
         <v>8080</v>
       </c>
-      <c r="C23">
+      <c r="C31" s="20">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B24">
+      <c r="B32" s="19">
         <v>8000</v>
       </c>
-      <c r="C24">
+      <c r="C32" s="20">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B25">
+      <c r="B33" s="19">
         <v>7800</v>
       </c>
-      <c r="C25">
+      <c r="C33" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B26">
+      <c r="B34" s="19">
         <v>7500</v>
       </c>
-      <c r="C26">
+      <c r="C34" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B27">
+      <c r="B35" s="19">
         <v>7440</v>
       </c>
-      <c r="C27">
+      <c r="C35" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B28">
+      <c r="B36" s="19">
         <v>7200</v>
       </c>
-      <c r="C28">
+      <c r="C36" s="20">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B29">
+      <c r="B37" s="19">
         <v>7030</v>
       </c>
-      <c r="C29">
+      <c r="C37" s="20">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B30">
+      <c r="B38" s="19">
         <v>6810</v>
       </c>
-      <c r="C30">
+      <c r="C38" s="20">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B31">
+      <c r="B39" s="19">
         <v>6720</v>
       </c>
-      <c r="C31">
+      <c r="C39" s="20">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B32">
+      <c r="B40" s="19">
         <v>6640</v>
       </c>
-      <c r="C32">
+      <c r="C40" s="20">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B33">
+      <c r="B41" s="19">
         <v>6510</v>
       </c>
-      <c r="C33">
+      <c r="C41" s="20">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B34">
+      <c r="B42" s="19">
         <v>6340</v>
       </c>
-      <c r="C34">
+      <c r="C42" s="20">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B35">
+      <c r="B43" s="19">
         <v>6240</v>
       </c>
-      <c r="C35">
+      <c r="C43" s="20">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B36">
+      <c r="B44" s="19">
         <v>6150</v>
       </c>
-      <c r="C36">
+      <c r="C44" s="20">
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B37">
+      <c r="B45" s="19">
         <v>6040</v>
       </c>
-      <c r="C37">
+      <c r="C45" s="20">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B38">
+      <c r="B46" s="19">
         <v>5920</v>
       </c>
-      <c r="C38">
+      <c r="C46" s="20">
         <v>-0.09</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B39">
+      <c r="B47" s="19">
         <v>5880</v>
       </c>
-      <c r="C39">
+      <c r="C47" s="20">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B40">
+      <c r="B48" s="19">
         <v>5770</v>
       </c>
-      <c r="C40">
+      <c r="C48" s="20">
         <v>-0.11</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B41">
+      <c r="B49" s="19">
         <v>5720</v>
       </c>
-      <c r="C41">
+      <c r="C49" s="20">
         <v>-0.12</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B42">
+      <c r="B50" s="19">
         <v>5680</v>
       </c>
-      <c r="C42">
+      <c r="C50" s="20">
         <v>-0.13</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B43">
+      <c r="B51" s="19">
         <v>5660</v>
       </c>
-      <c r="C43">
+      <c r="C51" s="20">
         <v>-0.13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B44">
+      <c r="B52" s="19">
         <v>5590</v>
       </c>
-      <c r="C44">
+      <c r="C52" s="20">
         <v>-0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B45">
+      <c r="B53" s="19">
         <v>5530</v>
       </c>
-      <c r="C45">
+      <c r="C53" s="20">
         <v>-0.16</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B46">
+      <c r="B54" s="19">
         <v>5490</v>
       </c>
-      <c r="C46">
+      <c r="C54" s="20">
         <v>-0.17</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B47">
+      <c r="B55" s="19">
         <v>5340</v>
       </c>
-      <c r="C47">
+      <c r="C55" s="20">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B48">
+      <c r="B56" s="19">
         <v>5280</v>
       </c>
-      <c r="C48">
+      <c r="C56" s="20">
         <v>-0.22</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B49">
+      <c r="B57" s="19">
         <v>5170</v>
       </c>
-      <c r="C49">
+      <c r="C57" s="20">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B50">
+      <c r="B58" s="19">
         <v>5040</v>
       </c>
-      <c r="C50">
+      <c r="C58" s="20">
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B51">
+      <c r="B59" s="19">
         <v>4840</v>
       </c>
-      <c r="C51">
+      <c r="C59" s="20">
         <v>-0.41</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B52">
+      <c r="B60" s="19">
         <v>4620</v>
       </c>
-      <c r="C52">
+      <c r="C60" s="20">
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B53">
+      <c r="B61" s="19">
         <v>4450</v>
       </c>
-      <c r="C53">
+      <c r="C61" s="20">
         <v>-0.67</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B54">
+      <c r="B62" s="19">
         <v>4200</v>
       </c>
-      <c r="C54">
+      <c r="C62" s="20">
         <v>-0.86</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B55">
+      <c r="B63" s="19">
         <v>4050</v>
       </c>
-      <c r="C55">
+      <c r="C63" s="20">
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B56">
+      <c r="B64" s="19">
         <v>3970</v>
       </c>
-      <c r="C56">
+      <c r="C64" s="20">
         <v>-1.1100000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B57">
+      <c r="B65" s="19">
         <v>3880</v>
       </c>
-      <c r="C57">
+      <c r="C65" s="20">
         <v>-1.25</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B58">
+      <c r="B66" s="19">
         <v>3850</v>
       </c>
-      <c r="C58">
+      <c r="C66" s="20">
         <v>-1.3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B59">
+      <c r="B67" s="19">
         <v>3680</v>
       </c>
-      <c r="C59">
+      <c r="C67" s="20">
         <v>-1.53</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B60">
+      <c r="B68" s="19">
         <v>3550</v>
       </c>
-      <c r="C60">
+      <c r="C68" s="20">
         <v>-1.65</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B61">
+      <c r="B69" s="19">
         <v>3400</v>
       </c>
-      <c r="C61">
+      <c r="C69" s="20">
         <v>-1.97</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B62">
+      <c r="B70" s="19">
         <v>3200</v>
       </c>
-      <c r="C62">
+      <c r="C70" s="20">
         <v>-2.59</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B63">
+      <c r="B71" s="19">
         <v>3050</v>
       </c>
-      <c r="C63">
+      <c r="C71" s="20">
         <v>-3.28</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B64">
+      <c r="B72" s="19">
         <v>2800</v>
       </c>
-      <c r="C64">
+      <c r="C72" s="20">
         <v>-4.3600000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B65">
+      <c r="B73" s="19">
         <v>2650</v>
       </c>
-      <c r="C65">
+      <c r="C73" s="20">
         <v>-5.0599999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B66">
+      <c r="B74" s="19">
         <v>2570</v>
       </c>
-      <c r="C66">
+      <c r="C74" s="20">
         <v>-5.66</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B67">
+      <c r="B75" s="22">
         <v>2450</v>
       </c>
-      <c r="C67">
+      <c r="C75" s="23">
         <v>-5.73</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D01BDD9-1727-4CA0-BE7C-5AA23A771920}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="34"/>
+      <c r="H1" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="42"/>
+      <c r="L1" s="49">
+        <v>0</v>
+      </c>
+      <c r="M1" s="50"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="K2" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="30">
+        <v>-7</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30">
+        <v>-5</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2">
+        <v>-6.4</v>
+      </c>
+      <c r="L3" s="45">
+        <v>-10</v>
+      </c>
+      <c r="M3" s="46">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="24">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C4" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="2">
+        <v>-7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-6.4</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-6.2</v>
+      </c>
+      <c r="L4" s="45"/>
+      <c r="M4" s="46"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="C5" s="3">
+        <v>13</v>
+      </c>
+      <c r="D5" s="55"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-2</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-6.2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-6</v>
+      </c>
+      <c r="L5" s="45"/>
+      <c r="M5" s="46"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>14</v>
+      </c>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-6</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-5.9</v>
+      </c>
+      <c r="L6" s="45"/>
+      <c r="M6" s="46"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-5.9</v>
+      </c>
+      <c r="K7" s="2">
+        <v>-5.7</v>
+      </c>
+      <c r="L7" s="45"/>
+      <c r="M7" s="46"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="3">
+        <v>-0.3</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-5.7</v>
+      </c>
+      <c r="K8" s="2">
+        <v>-5.3</v>
+      </c>
+      <c r="L8" s="45"/>
+      <c r="M8" s="46"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="7">
+        <v>8</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="7">
+        <v>7.7</v>
+      </c>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32">
+        <v>-0.4</v>
+      </c>
+      <c r="I9" s="31">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="J9" s="32">
+        <v>-5.3</v>
+      </c>
+      <c r="K9" s="44">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L9" s="47"/>
+      <c r="M9" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L3:L9"/>
+    <mergeCell ref="M3:M9"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBB8EB4-191D-4D0F-84F6-3FC58BE6703D}">
+  <dimension ref="A1:D57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3">
+        <v>54000</v>
+      </c>
+      <c r="C3">
+        <v>-10</v>
+      </c>
+      <c r="D3">
+        <v>846000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4">
+        <v>45000</v>
+      </c>
+      <c r="C4">
+        <v>-8.8000000000000007</v>
+      </c>
+      <c r="D4">
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5">
+        <v>43300</v>
+      </c>
+      <c r="C5">
+        <v>-8.6</v>
+      </c>
+      <c r="D5">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6">
+        <v>40600</v>
+      </c>
+      <c r="C6">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="D6">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7">
+        <v>37800</v>
+      </c>
+      <c r="C7">
+        <v>-7.7</v>
+      </c>
+      <c r="D7">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8">
+        <v>29200</v>
+      </c>
+      <c r="C8">
+        <v>-6</v>
+      </c>
+      <c r="D8">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9">
+        <v>23000</v>
+      </c>
+      <c r="C9">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="D9">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <v>21000</v>
+      </c>
+      <c r="C10">
+        <v>-3.8</v>
+      </c>
+      <c r="D10">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>17600</v>
+      </c>
+      <c r="C11">
+        <v>-2.6</v>
+      </c>
+      <c r="D11">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <v>15200</v>
+      </c>
+      <c r="C12">
+        <v>-1.6</v>
+      </c>
+      <c r="D12">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>14300</v>
+      </c>
+      <c r="C13">
+        <v>-1.2</v>
+      </c>
+      <c r="D13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14">
+        <v>13500</v>
+      </c>
+      <c r="C14">
+        <v>-0.84</v>
+      </c>
+      <c r="D14">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15">
+        <v>12300</v>
+      </c>
+      <c r="C15">
+        <v>-0.23</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16">
+        <v>11400</v>
+      </c>
+      <c r="C16">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D16">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17">
+        <v>9600</v>
+      </c>
+      <c r="C17">
+        <v>1.4</v>
+      </c>
+      <c r="D17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18">
+        <v>9330</v>
+      </c>
+      <c r="C18">
+        <v>1.6</v>
+      </c>
+      <c r="D18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19">
+        <v>9040</v>
+      </c>
+      <c r="C19">
+        <v>1.8</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20">
+        <v>8750</v>
+      </c>
+      <c r="C20">
+        <v>2.1</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21">
+        <v>8480</v>
+      </c>
+      <c r="C21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22">
+        <v>8310</v>
+      </c>
+      <c r="C22">
+        <v>2.4</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23">
+        <v>7920</v>
+      </c>
+      <c r="C23">
+        <v>2.7</v>
+      </c>
+      <c r="D23">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24">
+        <v>7350</v>
+      </c>
+      <c r="C24">
+        <v>3.2</v>
+      </c>
+      <c r="D24">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25">
+        <v>7050</v>
+      </c>
+      <c r="C25">
+        <v>3.5</v>
+      </c>
+      <c r="D25">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26">
+        <v>6850</v>
+      </c>
+      <c r="C26">
+        <v>3.7</v>
+      </c>
+      <c r="D26">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27">
+        <v>6700</v>
+      </c>
+      <c r="C27">
+        <v>3.8</v>
+      </c>
+      <c r="D27">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28">
+        <v>6550</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29">
+        <v>6400</v>
+      </c>
+      <c r="C29">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D29">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30">
+        <v>6300</v>
+      </c>
+      <c r="C30">
+        <v>4.2</v>
+      </c>
+      <c r="D30">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31">
+        <v>6050</v>
+      </c>
+      <c r="C31">
+        <v>4.5</v>
+      </c>
+      <c r="D31">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32">
+        <v>5930</v>
+      </c>
+      <c r="C32">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D32">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33">
+        <v>5800</v>
+      </c>
+      <c r="C33">
+        <v>4.8</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34">
+        <v>5660</v>
+      </c>
+      <c r="C34">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D34">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35">
+        <v>5440</v>
+      </c>
+      <c r="C35">
+        <v>5.2</v>
+      </c>
+      <c r="D35">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36">
+        <v>5240</v>
+      </c>
+      <c r="C36">
+        <v>5.4</v>
+      </c>
+      <c r="D36">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37">
+        <v>5110</v>
+      </c>
+      <c r="C37">
+        <v>5.6</v>
+      </c>
+      <c r="D37">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38">
+        <v>4960</v>
+      </c>
+      <c r="C38">
+        <v>5.8</v>
+      </c>
+      <c r="D38">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39">
+        <v>4800</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40">
+        <v>4600</v>
+      </c>
+      <c r="C40">
+        <v>6.3</v>
+      </c>
+      <c r="D40">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41">
+        <v>4400</v>
+      </c>
+      <c r="C41">
+        <v>6.6</v>
+      </c>
+      <c r="D41">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42">
+        <v>4000</v>
+      </c>
+      <c r="C42">
+        <v>7.3</v>
+      </c>
+      <c r="D42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43">
+        <v>3750</v>
+      </c>
+      <c r="C43">
+        <v>7.7</v>
+      </c>
+      <c r="D43">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44">
+        <v>3700</v>
+      </c>
+      <c r="C44">
+        <v>7.8</v>
+      </c>
+      <c r="D44">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45">
+        <v>3600</v>
+      </c>
+      <c r="C45">
+        <v>7.9</v>
+      </c>
+      <c r="D45">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46">
+        <v>3500</v>
+      </c>
+      <c r="C46">
+        <v>8.1</v>
+      </c>
+      <c r="D46">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47">
+        <v>3400</v>
+      </c>
+      <c r="C47">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D47">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48">
+        <v>3200</v>
+      </c>
+      <c r="C48">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D48">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49">
+        <v>3100</v>
+      </c>
+      <c r="C49">
+        <v>8.9</v>
+      </c>
+      <c r="D49">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50">
+        <v>2900</v>
+      </c>
+      <c r="C50">
+        <v>9.4</v>
+      </c>
+      <c r="D50">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51">
+        <v>2700</v>
+      </c>
+      <c r="C51">
+        <v>9.9</v>
+      </c>
+      <c r="D51">
+        <v>9.2999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52">
+        <v>2600</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53">
+        <v>2200</v>
+      </c>
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54">
+        <v>1500</v>
+      </c>
+      <c r="C54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54">
+        <v>2.5999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55">
+        <v>1400</v>
+      </c>
+      <c r="C55" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55">
+        <v>1.7000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56">
+        <v>1000</v>
+      </c>
+      <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56">
+        <v>2.0999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>98</v>
+      </c>
+      <c r="B57">
+        <v>800</v>
+      </c>
+      <c r="C57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57">
+        <v>5.4999999999999999E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C75D0E-68A4-460E-A813-D168EF86652D}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G3:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="G1" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3">
+        <v>5010</v>
+      </c>
+      <c r="C3">
+        <v>0.7</v>
+      </c>
+      <c r="D3">
+        <v>127</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4">
+        <v>4870</v>
+      </c>
+      <c r="C4">
+        <v>0.6</v>
+      </c>
+      <c r="D4">
+        <v>113</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5">
+        <v>4720</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>96</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5">
+        <v>-0.4</v>
+      </c>
+      <c r="H5">
+        <v>-1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6">
+        <v>4580</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+      <c r="D6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7">
+        <v>4460</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8">
+        <v>4210</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9">
+        <v>4010</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10">
+        <v>3780</v>
+      </c>
+      <c r="C10">
+        <v>-0.2</v>
+      </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11">
+        <v>3660</v>
+      </c>
+      <c r="C11">
+        <v>-0.4</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12">
+        <v>3600</v>
+      </c>
+      <c r="C12">
+        <v>-0.5</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13">
+        <v>3500</v>
+      </c>
+      <c r="C13">
+        <v>-0.6</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14">
+        <v>3300</v>
+      </c>
+      <c r="C14">
+        <v>-0.7</v>
+      </c>
+      <c r="D14">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15">
+        <v>3100</v>
+      </c>
+      <c r="C15">
+        <v>-0.75</v>
+      </c>
+      <c r="D15">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16">
+        <v>2950</v>
+      </c>
+      <c r="C16">
+        <v>-0.8</v>
+      </c>
+      <c r="D16">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17">
+        <v>2800</v>
+      </c>
+      <c r="C17">
+        <v>-0.9</v>
+      </c>
+      <c r="D17">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="26">
+        <v>-0.98571428571428599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="26">
+        <v>-1.0660714285714299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="26">
+        <v>-1.14642857142857</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3A82B3-0686-43FA-BFF1-FA5E0E910E8B}">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G3:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="G1" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3">
+        <v>21000</v>
+      </c>
+      <c r="C3">
+        <v>-6.4</v>
+      </c>
+      <c r="D3">
+        <v>320000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3">
+        <v>-6.4</v>
+      </c>
+      <c r="H3">
+        <v>-6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4">
+        <v>16000</v>
+      </c>
+      <c r="C4">
+        <v>-6.4</v>
+      </c>
+      <c r="D4">
+        <v>280000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4">
+        <v>-6.2</v>
+      </c>
+      <c r="H4">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5">
+        <v>14000</v>
+      </c>
+      <c r="C5">
+        <v>-6.4</v>
+      </c>
+      <c r="D5">
+        <v>220000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5">
+        <v>-6</v>
+      </c>
+      <c r="H5">
+        <v>-5.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6">
+        <v>12800</v>
+      </c>
+      <c r="C6">
+        <v>-6.3</v>
+      </c>
+      <c r="D6">
+        <v>180000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6">
+        <v>-5.9</v>
+      </c>
+      <c r="H6">
+        <v>-5.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7">
+        <v>11500</v>
+      </c>
+      <c r="C7">
+        <v>-6.3</v>
+      </c>
+      <c r="D7">
+        <v>140000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7">
+        <v>-5.7</v>
+      </c>
+      <c r="H7">
+        <v>-5.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8">
+        <v>11000</v>
+      </c>
+      <c r="C8">
+        <v>-6.3</v>
+      </c>
+      <c r="D8">
+        <v>98000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8">
+        <v>-5.3</v>
+      </c>
+      <c r="H8" s="27">
+        <v>-5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <v>10500</v>
+      </c>
+      <c r="C9">
+        <v>-6.3</v>
+      </c>
+      <c r="D9">
+        <v>82000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10">
+        <v>10000</v>
+      </c>
+      <c r="C10">
+        <v>-6.2</v>
+      </c>
+      <c r="D10">
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11">
+        <v>9700</v>
+      </c>
+      <c r="C11">
+        <v>-6.2</v>
+      </c>
+      <c r="D11">
+        <v>61000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12">
+        <v>9400</v>
+      </c>
+      <c r="C12">
+        <v>-6.2</v>
+      </c>
+      <c r="D12">
+        <v>50600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13">
+        <v>9100</v>
+      </c>
+      <c r="C13">
+        <v>-6.2</v>
+      </c>
+      <c r="D13">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14">
+        <v>8900</v>
+      </c>
+      <c r="C14">
+        <v>-6.2</v>
+      </c>
+      <c r="D14">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15">
+        <v>8300</v>
+      </c>
+      <c r="C15">
+        <v>-6.1</v>
+      </c>
+      <c r="D15">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16">
+        <v>7500</v>
+      </c>
+      <c r="C16">
+        <v>-6</v>
+      </c>
+      <c r="D16">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17">
+        <v>7200</v>
+      </c>
+      <c r="C17">
+        <v>-6</v>
+      </c>
+      <c r="D17">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18">
+        <v>6800</v>
+      </c>
+      <c r="C18">
+        <v>-5.9</v>
+      </c>
+      <c r="D18">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19">
+        <v>6150</v>
+      </c>
+      <c r="C19">
+        <v>-5.9</v>
+      </c>
+      <c r="D19">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20">
+        <v>5800</v>
+      </c>
+      <c r="C20">
+        <v>-5.9</v>
+      </c>
+      <c r="D20">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21">
+        <v>5500</v>
+      </c>
+      <c r="C21">
+        <v>-5.8</v>
+      </c>
+      <c r="D21">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22">
+        <v>5100</v>
+      </c>
+      <c r="C22">
+        <v>-5.8</v>
+      </c>
+      <c r="D22">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23">
+        <v>5050</v>
+      </c>
+      <c r="C23">
+        <v>-5.7</v>
+      </c>
+      <c r="D23">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24">
+        <v>4900</v>
+      </c>
+      <c r="C24">
+        <v>-5.7</v>
+      </c>
+      <c r="D24">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25">
+        <v>4700</v>
+      </c>
+      <c r="C25">
+        <v>-5.6</v>
+      </c>
+      <c r="D25">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26">
+        <v>4500</v>
+      </c>
+      <c r="C26">
+        <v>-5.6</v>
+      </c>
+      <c r="D26">
+        <v>15200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27">
+        <v>4300</v>
+      </c>
+      <c r="C27">
+        <v>-5.6</v>
+      </c>
+      <c r="D27">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28">
+        <v>4100</v>
+      </c>
+      <c r="C28">
+        <v>-5.5</v>
+      </c>
+      <c r="D28">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29">
+        <v>3750</v>
+      </c>
+      <c r="C29">
+        <v>-5.5</v>
+      </c>
+      <c r="D29">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30">
+        <v>3660</v>
+      </c>
+      <c r="C30">
+        <v>-5.3</v>
+      </c>
+      <c r="D30">
+        <v>50600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31">
+        <v>3600</v>
+      </c>
+      <c r="C31">
+        <v>-5.3</v>
+      </c>
+      <c r="D31">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32">
+        <v>3500</v>
+      </c>
+      <c r="C32">
+        <v>-5.3</v>
+      </c>
+      <c r="D32">
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33">
+        <v>3300</v>
+      </c>
+      <c r="C33">
+        <v>-5.3</v>
+      </c>
+      <c r="D33">
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34">
+        <v>3100</v>
+      </c>
+      <c r="C34">
+        <v>-5.2</v>
+      </c>
+      <c r="D34">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35">
+        <v>2950</v>
+      </c>
+      <c r="C35">
+        <v>-5.2</v>
+      </c>
+      <c r="D35">
+        <v>58000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="26">
+        <v>-5.1866666666666701</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="26">
+        <v>-5.1638095238095199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="26">
+        <v>-5.1409523809523803</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>158</v>
+      </c>
+      <c r="C39" s="26">
+        <v>-5.1180952380952398</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Automatic luminosity class assignment
data is fetched from magnitudes.csv
ERROR: function finds correct ranges but in an incorrect class (e.g. III instead of V)
</commit_message>
<xml_diff>
--- a/Authorative Table.xlsx
+++ b/Authorative Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNITY\Orbit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hunor\UNITY\Orbit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD17515-CE7A-48DA-8230-F333D041509A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E7C421-1F8F-4979-819A-7A75F5BB35AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4F9C6455-CBDE-45B2-AE91-212659DAF4F4}"/>
+    <workbookView xWindow="7200" yWindow="3150" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{4F9C6455-CBDE-45B2-AE91-212659DAF4F4}"/>
   </bookViews>
   <sheets>
     <sheet name="bolometric correction" sheetId="1" r:id="rId1"/>
@@ -31,8 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="168">
   <si>
     <t>Spectral Type</t>
   </si>
@@ -535,6 +533,15 @@
   </si>
   <si>
     <t>ű</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Infinity</t>
   </si>
 </sst>
 </file>
@@ -542,7 +549,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -584,52 +591,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="29">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -898,23 +865,14 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -924,86 +882,10 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1020,11 +902,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="double">
@@ -1034,13 +916,13 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1049,74 +931,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1126,23 +1008,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -2768,67 +2637,67 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14"/>
-      <c r="F1" s="12" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="F1" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="19" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12">
         <v>-4.7474999999999996</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>-4.8</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>-3.06</v>
       </c>
       <c r="I3">
@@ -2846,21 +2715,21 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15">
         <v>-4.5459523809523796</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>-3.03</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>-0.38</v>
       </c>
       <c r="I4">
@@ -2879,21 +2748,21 @@
         <v>-2.7649999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15">
         <v>-4.3444047619047703</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>-0.24</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>0</v>
       </c>
       <c r="I5">
@@ -2912,21 +2781,21 @@
         <v>-0.14399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15">
         <v>-4.1428571428571397</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>-0.01</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>-0.08</v>
       </c>
       <c r="I6">
@@ -2945,21 +2814,21 @@
         <v>-3.1000000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15">
         <v>-3.9413095238095202</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>-0.09</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>-0.21</v>
       </c>
       <c r="I7">
@@ -2978,21 +2847,21 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20">
+      <c r="B8" s="14"/>
+      <c r="C8" s="15">
         <v>-3.7397619047619002</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>-0.22</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>-1.25</v>
       </c>
       <c r="I8">
@@ -3011,21 +2880,21 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20">
+      <c r="B9" s="14"/>
+      <c r="C9" s="15">
         <v>-3.53821428571429</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>-1.3</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <v>-5.73</v>
       </c>
       <c r="I9">
@@ -3044,729 +2913,729 @@
         <v>-5.73</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="14">
         <v>34000</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="15">
         <v>-3.2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="14">
         <v>32000</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="15">
         <v>-3.06</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="14">
         <v>31500</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="15">
         <v>-3.03</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="14">
         <v>29000</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="15">
         <v>-2.87</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="14">
         <v>26000</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="15">
         <v>-2.61</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="14">
         <v>24800</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="15">
         <v>-2.4300000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="14">
         <v>20600</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="15">
         <v>-2.06</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="14">
         <v>18500</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="15">
         <v>-1.79</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="14">
         <v>17000</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="15">
         <v>-1.58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="14">
         <v>16700</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="15">
         <v>-1.53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="14">
         <v>15700</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="15">
         <v>-1.37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="14">
         <v>14500</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="15">
         <v>-1.1599999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="14">
         <v>14000</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="15">
         <v>-1.07</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="14">
         <v>12500</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="15">
         <v>-0.79</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="14">
         <v>10700</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="15">
         <v>-0.44</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="14">
         <v>10400</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="15">
         <v>-0.38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="14">
         <v>9700</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="15">
         <v>-0.24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="14">
         <v>9200</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="15">
         <v>-0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="14">
         <v>8840</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="15">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="14">
         <v>8550</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="15">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="14">
         <v>8270</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="15">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="14">
         <v>8080</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="15">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="19">
+      <c r="B32" s="14">
         <v>8000</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="15">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="14">
         <v>7800</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="19">
+      <c r="B34" s="14">
         <v>7500</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="19">
+      <c r="B35" s="14">
         <v>7440</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="19">
+      <c r="B36" s="14">
         <v>7200</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="15">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="19">
+      <c r="B37" s="14">
         <v>7030</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="15">
         <v>-0.01</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="19">
+      <c r="B38" s="14">
         <v>6810</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="15">
         <v>-0.02</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="14">
         <v>6720</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="15">
         <v>-0.03</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="19">
+      <c r="B40" s="14">
         <v>6640</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="15">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="19">
+      <c r="B41" s="14">
         <v>6510</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="15">
         <v>-0.04</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B42" s="14">
         <v>6340</v>
       </c>
-      <c r="C42" s="20">
+      <c r="C42" s="15">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="19">
+      <c r="B43" s="14">
         <v>6240</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="15">
         <v>-0.06</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="19">
+      <c r="B44" s="14">
         <v>6150</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="15">
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="18" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="19">
+      <c r="B45" s="14">
         <v>6040</v>
       </c>
-      <c r="C45" s="20">
+      <c r="C45" s="15">
         <v>-0.08</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="18" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="19">
+      <c r="B46" s="14">
         <v>5920</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C46" s="15">
         <v>-0.09</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="18" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="14">
         <v>5880</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="15">
         <v>-0.1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="14">
         <v>5770</v>
       </c>
-      <c r="C48" s="20">
+      <c r="C48" s="15">
         <v>-0.11</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="14">
         <v>5720</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C49" s="15">
         <v>-0.12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="19">
+      <c r="B50" s="14">
         <v>5680</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C50" s="15">
         <v>-0.13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="18" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="14">
         <v>5660</v>
       </c>
-      <c r="C51" s="20">
+      <c r="C51" s="15">
         <v>-0.13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="18" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="19">
+      <c r="B52" s="14">
         <v>5590</v>
       </c>
-      <c r="C52" s="20">
+      <c r="C52" s="15">
         <v>-0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="18" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="19">
+      <c r="B53" s="14">
         <v>5530</v>
       </c>
-      <c r="C53" s="20">
+      <c r="C53" s="15">
         <v>-0.16</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="18" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B54" s="19">
+      <c r="B54" s="14">
         <v>5490</v>
       </c>
-      <c r="C54" s="20">
+      <c r="C54" s="15">
         <v>-0.17</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="18" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="19">
+      <c r="B55" s="14">
         <v>5340</v>
       </c>
-      <c r="C55" s="20">
+      <c r="C55" s="15">
         <v>-0.21</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="18" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="19">
+      <c r="B56" s="14">
         <v>5280</v>
       </c>
-      <c r="C56" s="20">
+      <c r="C56" s="15">
         <v>-0.22</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="18" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="19">
+      <c r="B57" s="14">
         <v>5170</v>
       </c>
-      <c r="C57" s="20">
+      <c r="C57" s="15">
         <v>-0.26</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="18" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="19">
+      <c r="B58" s="14">
         <v>5040</v>
       </c>
-      <c r="C58" s="20">
+      <c r="C58" s="15">
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="18" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="19">
+      <c r="B59" s="14">
         <v>4840</v>
       </c>
-      <c r="C59" s="20">
+      <c r="C59" s="15">
         <v>-0.41</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="18" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="19">
+      <c r="B60" s="14">
         <v>4620</v>
       </c>
-      <c r="C60" s="20">
+      <c r="C60" s="15">
         <v>-0.55000000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="19">
+      <c r="B61" s="14">
         <v>4450</v>
       </c>
-      <c r="C61" s="20">
+      <c r="C61" s="15">
         <v>-0.67</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="18" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B62" s="19">
+      <c r="B62" s="14">
         <v>4200</v>
       </c>
-      <c r="C62" s="20">
+      <c r="C62" s="15">
         <v>-0.86</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="18" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="19">
+      <c r="B63" s="14">
         <v>4050</v>
       </c>
-      <c r="C63" s="20">
+      <c r="C63" s="15">
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="18" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="19">
+      <c r="B64" s="14">
         <v>3970</v>
       </c>
-      <c r="C64" s="20">
+      <c r="C64" s="15">
         <v>-1.1100000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="18" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="19">
+      <c r="B65" s="14">
         <v>3880</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="15">
         <v>-1.25</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="18" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="19">
+      <c r="B66" s="14">
         <v>3850</v>
       </c>
-      <c r="C66" s="20">
+      <c r="C66" s="15">
         <v>-1.3</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="18" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="19">
+      <c r="B67" s="14">
         <v>3680</v>
       </c>
-      <c r="C67" s="20">
+      <c r="C67" s="15">
         <v>-1.53</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="18" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="19">
+      <c r="B68" s="14">
         <v>3550</v>
       </c>
-      <c r="C68" s="20">
+      <c r="C68" s="15">
         <v>-1.65</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="18" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B69" s="19">
+      <c r="B69" s="14">
         <v>3400</v>
       </c>
-      <c r="C69" s="20">
+      <c r="C69" s="15">
         <v>-1.97</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="18" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B70" s="19">
+      <c r="B70" s="14">
         <v>3200</v>
       </c>
-      <c r="C70" s="20">
+      <c r="C70" s="15">
         <v>-2.59</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B71" s="19">
+      <c r="B71" s="14">
         <v>3050</v>
       </c>
-      <c r="C71" s="20">
+      <c r="C71" s="15">
         <v>-3.28</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="18" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="19">
+      <c r="B72" s="14">
         <v>2800</v>
       </c>
-      <c r="C72" s="20">
+      <c r="C72" s="15">
         <v>-4.3600000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="18" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B73" s="19">
+      <c r="B73" s="14">
         <v>2650</v>
       </c>
-      <c r="C73" s="20">
+      <c r="C73" s="15">
         <v>-5.0599999999999996</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="18" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="19">
+      <c r="B74" s="14">
         <v>2570</v>
       </c>
-      <c r="C74" s="20">
+      <c r="C74" s="15">
         <v>-5.66</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="21" t="s">
+    <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B75" s="22">
+      <c r="B75" s="17">
         <v>2450</v>
       </c>
-      <c r="C75" s="23">
+      <c r="C75" s="18">
         <v>-5.73</v>
       </c>
     </row>
@@ -3783,212 +3652,279 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D01BDD9-1727-4CA0-BE7C-5AA23A771920}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
       <c r="B1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="34"/>
+      <c r="E1" s="35"/>
       <c r="F1" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="35" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="35"/>
+      <c r="J1" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" s="35"/>
+      <c r="N1" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="49">
+      <c r="O1" s="35"/>
+      <c r="P1" s="33">
         <v>0</v>
       </c>
-      <c r="M1" s="50"/>
-    </row>
-    <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8"/>
-      <c r="B2" s="36" t="s">
+      <c r="Q1" s="35"/>
+    </row>
+    <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="L2" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="26" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="N2" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="P2" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q2" s="48" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="30">
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="44">
+        <v>-5</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="44">
+        <v>-5.5</v>
+      </c>
+      <c r="K3" s="45">
+        <v>-5</v>
+      </c>
+      <c r="L3" s="53">
+        <v>-6.4</v>
+      </c>
+      <c r="M3" s="53">
+        <v>-5.5</v>
+      </c>
+      <c r="N3" s="2">
         <v>-7</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="30">
-        <v>-5</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2">
+      <c r="O3" s="3">
         <v>-6.4</v>
       </c>
-      <c r="L3" s="45">
+      <c r="P3" s="49">
         <v>-10</v>
       </c>
-      <c r="M3" s="46">
+      <c r="Q3" s="50">
         <v>-7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="24">
-        <v>9.8000000000000007</v>
+      <c r="B4" s="39">
+        <v>8</v>
       </c>
       <c r="C4" s="3">
         <v>12.5</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>8</v>
+      </c>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="2">
+        <v>-4.8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>-2</v>
+      </c>
+      <c r="L4" s="19">
+        <v>-5.8</v>
+      </c>
+      <c r="M4" s="19">
+        <v>-4.8</v>
+      </c>
+      <c r="N4" s="2">
         <v>-7</v>
       </c>
-      <c r="G4" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>-5</v>
-      </c>
-      <c r="I4" s="3">
-        <v>-2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>-6.4</v>
-      </c>
-      <c r="K4" s="2">
-        <v>-6.2</v>
-      </c>
-      <c r="L4" s="45"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="O4" s="3">
+        <v>-5.8</v>
+      </c>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="50"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>81</v>
       </c>
       <c r="B5" s="2">
-        <v>10.1</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3">
         <v>13</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="56"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="2">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="H5" s="1">
-        <v>-2</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="J5" s="1">
-        <v>-6.2</v>
-      </c>
-      <c r="K5" s="2">
-        <v>-6</v>
-      </c>
-      <c r="L5" s="45"/>
-      <c r="M5" s="46"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="19">
+        <v>1</v>
+      </c>
+      <c r="I5" s="19">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>-3</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="19">
+        <v>-5</v>
+      </c>
+      <c r="M5" s="19">
+        <v>-3</v>
+      </c>
+      <c r="N5" s="2">
+        <v>-7</v>
+      </c>
+      <c r="O5" s="3">
+        <v>-5</v>
+      </c>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="50"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
         <v>14</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="2">
         <v>3.2</v>
       </c>
       <c r="G6" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="J6" s="1">
-        <v>-6</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-5.9</v>
-      </c>
-      <c r="L6" s="45"/>
-      <c r="M6" s="46"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="19">
+        <v>1.3</v>
+      </c>
+      <c r="I6" s="19">
+        <v>3.2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>-0.7</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="L6" s="19">
+        <v>-4.5</v>
+      </c>
+      <c r="M6" s="19">
+        <v>-0.7</v>
+      </c>
+      <c r="N6" s="2">
+        <v>-7</v>
+      </c>
+      <c r="O6" s="3">
+        <v>-4.5</v>
+      </c>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="50"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>15</v>
@@ -4003,99 +3939,137 @@
         <v>4.5</v>
       </c>
       <c r="G7" s="3">
-        <v>5.3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="J7" s="1">
-        <v>-5.9</v>
-      </c>
-      <c r="K7" s="2">
-        <v>-5.7</v>
-      </c>
-      <c r="L7" s="45"/>
-      <c r="M7" s="46"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="19">
+        <v>2</v>
+      </c>
+      <c r="I7" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
+      <c r="L7" s="19">
+        <v>-4</v>
+      </c>
+      <c r="M7" s="19">
+        <v>-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>-7</v>
+      </c>
+      <c r="O7" s="3">
+        <v>-4</v>
+      </c>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="50"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="2">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>15.5</v>
       </c>
       <c r="D8" s="2">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="E8" s="3">
         <v>8</v>
       </c>
       <c r="F8" s="2">
-        <v>5.3</v>
+        <v>3.6</v>
       </c>
       <c r="G8" s="3">
+        <v>10</v>
+      </c>
+      <c r="H8" s="19">
+        <v>1</v>
+      </c>
+      <c r="I8" s="19">
+        <v>3.6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="19">
+        <v>-4.5</v>
+      </c>
+      <c r="M8" s="19">
+        <v>-2</v>
+      </c>
+      <c r="N8" s="2">
+        <v>-7</v>
+      </c>
+      <c r="O8" s="3">
+        <v>-4.5</v>
+      </c>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="50"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4">
         <v>7.7</v>
       </c>
-      <c r="H8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>-0.3</v>
-      </c>
-      <c r="J8" s="1">
-        <v>-5.7</v>
-      </c>
-      <c r="K8" s="2">
-        <v>-5.3</v>
-      </c>
-      <c r="L8" s="45"/>
-      <c r="M8" s="46"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="7">
-        <v>8</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="7">
-        <v>7.7</v>
-      </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32">
-        <v>-0.4</v>
-      </c>
-      <c r="I9" s="31">
+      <c r="G9" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="4">
+        <v>-2.5</v>
+      </c>
+      <c r="K9" s="6">
         <v>-1.1499999999999999</v>
       </c>
-      <c r="J9" s="32">
-        <v>-5.3</v>
-      </c>
-      <c r="K9" s="44">
-        <v>-5.0999999999999996</v>
-      </c>
-      <c r="L9" s="47"/>
-      <c r="M9" s="48"/>
+      <c r="L9" s="5">
+        <v>-4.5</v>
+      </c>
+      <c r="M9" s="5">
+        <v>-2.5</v>
+      </c>
+      <c r="N9" s="4">
+        <v>-7</v>
+      </c>
+      <c r="O9" s="46">
+        <v>-4.5</v>
+      </c>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="J1:K1"/>
+  <mergeCells count="10">
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P3:P9"/>
+    <mergeCell ref="Q3:Q9"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L3:L9"/>
-    <mergeCell ref="M3:M9"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4110,23 +4084,23 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -4140,7 +4114,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -4154,7 +4128,7 @@
         <v>846000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -4168,7 +4142,7 @@
         <v>275000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -4182,7 +4156,7 @@
         <v>220000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -4196,7 +4170,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -4210,7 +4184,7 @@
         <v>95000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -4224,7 +4198,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -4238,7 +4212,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -4252,7 +4226,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -4266,7 +4240,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -4280,7 +4254,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -4294,7 +4268,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -4308,7 +4282,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -4322,7 +4296,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -4336,7 +4310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -4350,7 +4324,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -4364,7 +4338,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -4378,7 +4352,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -4392,7 +4366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -4406,7 +4380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -4420,7 +4394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -4434,7 +4408,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -4448,7 +4422,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -4462,7 +4436,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>125</v>
       </c>
@@ -4476,7 +4450,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -4490,7 +4464,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -4504,7 +4478,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -4518,7 +4492,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -4532,7 +4506,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -4546,7 +4520,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -4560,7 +4534,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -4574,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -4588,7 +4562,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -4602,7 +4576,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -4616,7 +4590,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>136</v>
       </c>
@@ -4630,7 +4604,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -4644,7 +4618,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>138</v>
       </c>
@@ -4658,7 +4632,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -4672,7 +4646,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>140</v>
       </c>
@@ -4686,7 +4660,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -4700,7 +4674,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -4714,7 +4688,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>143</v>
       </c>
@@ -4728,7 +4702,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -4742,7 +4716,7 @@
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -4756,7 +4730,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -4770,7 +4744,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -4784,7 +4758,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -4798,7 +4772,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -4812,7 +4786,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>150</v>
       </c>
@@ -4826,7 +4800,7 @@
         <v>9.2999999999999992E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>151</v>
       </c>
@@ -4840,7 +4814,7 @@
         <v>7.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -4854,7 +4828,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>95</v>
       </c>
@@ -4868,7 +4842,7 @@
         <v>2.5999999999999998E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>96</v>
       </c>
@@ -4882,7 +4856,7 @@
         <v>1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>97</v>
       </c>
@@ -4896,7 +4870,7 @@
         <v>2.0999999999999999E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>98</v>
       </c>
@@ -4926,27 +4900,27 @@
       <selection activeCell="G5" sqref="G3:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -4966,7 +4940,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -4989,7 +4963,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -5012,7 +4986,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -5035,7 +5009,7 @@
         <v>-1.1499999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -5049,7 +5023,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -5063,7 +5037,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>138</v>
       </c>
@@ -5077,7 +5051,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>139</v>
       </c>
@@ -5091,7 +5065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -5105,7 +5079,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -5119,7 +5093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -5133,7 +5107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>144</v>
       </c>
@@ -5147,7 +5121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -5161,7 +5135,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -5175,7 +5149,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -5189,7 +5163,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -5203,27 +5177,27 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="20">
         <v>-0.98571428571428599</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="20">
         <v>-1.0660714285714299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="20">
         <v>-1.14642857142857</v>
       </c>
     </row>
@@ -5244,27 +5218,27 @@
       <selection activeCell="G8" sqref="G3:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="25"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -5284,7 +5258,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -5307,7 +5281,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>108</v>
       </c>
@@ -5330,7 +5304,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -5353,7 +5327,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -5376,7 +5350,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>111</v>
       </c>
@@ -5399,7 +5373,7 @@
         <v>-5.3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -5418,11 +5392,11 @@
       <c r="G8">
         <v>-5.3</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="21">
         <v>-5.0999999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -5436,7 +5410,7 @@
         <v>82000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -5450,7 +5424,7 @@
         <v>73000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
@@ -5464,7 +5438,7 @@
         <v>61000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -5478,7 +5452,7 @@
         <v>50600</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>117</v>
       </c>
@@ -5492,7 +5466,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>118</v>
       </c>
@@ -5506,7 +5480,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -5520,7 +5494,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
@@ -5534,7 +5508,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>124</v>
       </c>
@@ -5548,7 +5522,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
@@ -5562,7 +5536,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -5576,7 +5550,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>130</v>
       </c>
@@ -5590,7 +5564,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -5604,7 +5578,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -5618,7 +5592,7 @@
         <v>9800</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>134</v>
       </c>
@@ -5632,7 +5606,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -5646,7 +5620,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -5660,7 +5634,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -5674,7 +5648,7 @@
         <v>15200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -5688,7 +5662,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -5702,7 +5676,7 @@
         <v>18300</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -5716,7 +5690,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -5730,7 +5704,7 @@
         <v>50600</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -5744,7 +5718,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -5758,7 +5732,7 @@
         <v>53000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5772,7 +5746,7 @@
         <v>54000</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -5786,7 +5760,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -5800,35 +5774,35 @@
         <v>58000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="20">
         <v>-5.1866666666666701</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="20">
         <v>-5.1638095238095199</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="20">
         <v>-5.1409523809523803</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="20">
         <v>-5.1180952380952398</v>
       </c>
     </row>

</xml_diff>